<commit_message>
fix issues and add wishlist
</commit_message>
<xml_diff>
--- a/ecommerce.xlsx
+++ b/ecommerce.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KENIL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CE976A-2737-4AAC-87D9-E517B8258671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71619AD-EB02-4509-A44A-6B4CAFDECC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{785BB870-0898-4C38-870A-8BD1466B9A97}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="108">
   <si>
     <t>int</t>
   </si>
@@ -361,6 +361,15 @@
   </si>
   <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>Color_ID</t>
+  </si>
+  <si>
+    <t>Size_ID</t>
+  </si>
+  <si>
+    <t>Table :-Wishlist</t>
   </si>
 </sst>
 </file>
@@ -445,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -459,14 +468,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -783,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B9B093-5896-4E4E-AD3A-F02ED3F94AD7}">
-  <dimension ref="A1:E170"/>
+  <dimension ref="A1:E177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,13 +807,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1042,13 +1050,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -1203,13 +1211,13 @@
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -1317,13 +1325,13 @@
       <c r="E41" s="1"/>
     </row>
     <row r="43" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -1431,13 +1439,13 @@
       <c r="E51" s="1"/>
     </row>
     <row r="53" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
@@ -1491,16 +1499,16 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B58" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="7">
-        <v>10</v>
-      </c>
-      <c r="D58" s="7" t="s">
+      <c r="B58" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="5">
+        <v>10</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -1538,13 +1546,13 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B63" s="6"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
@@ -1601,16 +1609,16 @@
       <c r="A68" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="5">
         <v>255</v>
       </c>
-      <c r="D68" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E68" s="7" t="s">
+      <c r="D68" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1635,16 +1643,16 @@
       <c r="A70" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B70" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C70" s="7">
-        <v>10</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E70" s="7" t="s">
+      <c r="B70" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="5">
+        <v>10</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1652,16 +1660,16 @@
       <c r="A71" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C71" s="7">
-        <v>10</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E71" s="7" t="s">
+      <c r="B71" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="5">
+        <v>10</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1669,16 +1677,16 @@
       <c r="A72" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="5">
         <v>255</v>
       </c>
-      <c r="D72" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E72" s="7" t="s">
+      <c r="D72" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="5" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1686,16 +1694,16 @@
       <c r="A73" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B73" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C73" s="7">
-        <v>2</v>
-      </c>
-      <c r="D73" s="7" t="s">
+      <c r="B73" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="5">
+        <v>2</v>
+      </c>
+      <c r="D73" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E73" s="7" t="s">
+      <c r="E73" s="5" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1703,16 +1711,16 @@
       <c r="A74" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B74" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C74" s="7">
-        <v>10</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E74" s="7" t="s">
+      <c r="B74" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="5">
+        <v>10</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1754,16 +1762,16 @@
       <c r="A77" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B77" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="5">
         <v>50</v>
       </c>
-      <c r="D77" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E77" s="7" t="s">
+      <c r="D77" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="5" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1798,13 +1806,13 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A84" s="6" t="s">
+      <c r="A84" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6"/>
-      <c r="E84" s="6"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
@@ -1888,13 +1896,13 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A93" s="6" t="s">
+      <c r="A93" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
@@ -1948,16 +1956,16 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
+      <c r="A98" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B98" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C98" s="7">
+      <c r="C98" s="5">
         <v>20</v>
       </c>
-      <c r="D98" s="7" t="s">
+      <c r="D98" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E98" s="3" t="s">
@@ -1995,20 +2003,20 @@
       </c>
     </row>
     <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="6" t="s">
+      <c r="A102" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B102" s="6"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="6"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
     </row>
     <row r="103" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A103" s="8"/>
-      <c r="B103" s="8"/>
-      <c r="C103" s="8"/>
-      <c r="D103" s="8"/>
-      <c r="E103" s="8"/>
+      <c r="A103" s="6"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
@@ -2028,16 +2036,16 @@
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="7" t="s">
+      <c r="A105" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B105" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C105" s="7">
-        <v>10</v>
-      </c>
-      <c r="D105" s="7" t="s">
+      <c r="B105" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" s="5">
+        <v>10</v>
+      </c>
+      <c r="D105" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E105" s="3" t="s">
@@ -2045,19 +2053,19 @@
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="7" t="s">
+      <c r="A106" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B106" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C106" s="7">
-        <v>10</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E106" s="7" t="s">
+      <c r="C106" s="5">
+        <v>10</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E106" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2099,13 +2107,13 @@
       <c r="E109" s="3"/>
     </row>
     <row r="111" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A111" s="6" t="s">
+      <c r="A111" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B111" s="6"/>
-      <c r="C111" s="6"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="6"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
@@ -2125,16 +2133,16 @@
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="7" t="s">
+      <c r="A113" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B113" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C113" s="7">
-        <v>10</v>
-      </c>
-      <c r="D113" s="7" t="s">
+      <c r="B113" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C113" s="5">
+        <v>10</v>
+      </c>
+      <c r="D113" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E113" s="3" t="s">
@@ -2142,19 +2150,19 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="7" t="s">
+      <c r="A114" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B114" s="7" t="s">
+      <c r="B114" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C114" s="7">
-        <v>2</v>
-      </c>
-      <c r="D114" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E114" s="7" t="s">
+      <c r="C114" s="5">
+        <v>2</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E114" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2189,13 +2197,13 @@
       </c>
     </row>
     <row r="119" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A119" s="6" t="s">
+      <c r="A119" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B119" s="6"/>
-      <c r="C119" s="6"/>
-      <c r="D119" s="6"/>
-      <c r="E119" s="6"/>
+      <c r="B119" s="7"/>
+      <c r="C119" s="7"/>
+      <c r="D119" s="7"/>
+      <c r="E119" s="7"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
@@ -2267,13 +2275,13 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C125" s="3">
-        <v>10</v>
+        <v>255</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>19</v>
@@ -2284,7 +2292,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>0</v>
@@ -2301,131 +2309,114 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C127" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="C127" s="3">
+        <v>10</v>
+      </c>
       <c r="D127" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C128" s="3">
+        <v>10</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C129" s="3">
+        <v>10</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B128" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C128" s="3"/>
-      <c r="D128" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E128" s="3" t="s">
+      <c r="B131" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E131" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A131" s="6" t="s">
+    <row r="135" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A135" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B131" s="6"/>
-      <c r="C131" s="6"/>
-      <c r="D131" s="6"/>
-      <c r="E131" s="6"/>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
+      <c r="B135" s="7"/>
+      <c r="C135" s="7"/>
+      <c r="D135" s="7"/>
+      <c r="E135" s="7"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B137" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C137" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D133" s="2" t="s">
+      <c r="D137" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="2" t="s">
+      <c r="E137" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C134" s="3">
-        <v>10</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E134" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C135" s="3">
-        <v>10</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E135" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C136" s="3">
-        <v>10</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E136" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C137" s="3">
-        <v>10</v>
-      </c>
-      <c r="D137" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>0</v>
@@ -2437,12 +2428,12 @@
         <v>19</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>0</v>
@@ -2454,327 +2445,468 @@
         <v>19</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C140" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="C140" s="3">
+        <v>10</v>
+      </c>
       <c r="D140" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C141" s="3">
+        <v>10</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C142" s="3">
+        <v>10</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C143" s="3">
+        <v>10</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B141" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C141" s="3"/>
-      <c r="D141" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E141" s="3" t="s">
+      <c r="B145" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C145" s="3"/>
+      <c r="D145" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E145" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A144" s="6" t="s">
+    <row r="148" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A148" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B144" s="6"/>
-      <c r="C144" s="6"/>
-      <c r="D144" s="6"/>
-      <c r="E144" s="6"/>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
+      <c r="B148" s="7"/>
+      <c r="C148" s="7"/>
+      <c r="D148" s="7"/>
+      <c r="E148" s="7"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B150" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="C150" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D146" s="2" t="s">
+      <c r="D150" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E146" s="2" t="s">
+      <c r="E150" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C147" s="3">
-        <v>10</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E147" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C148" s="3">
-        <v>10</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E148" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C149" s="3">
-        <v>10</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C150" s="3">
-        <v>2</v>
-      </c>
-      <c r="D150" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E150" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C151" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="C151" s="3">
+        <v>10</v>
+      </c>
       <c r="D151" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C152" s="3">
+        <v>10</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C153" s="3">
+        <v>10</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C154" s="3">
+        <v>2</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C155" s="3"/>
+      <c r="D155" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B152" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C152" s="3"/>
-      <c r="D152" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E152" s="3" t="s">
+      <c r="B156" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C156" s="3"/>
+      <c r="D156" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E156" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A155" s="6" t="s">
+    <row r="159" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A159" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B155" s="6"/>
-      <c r="C155" s="6"/>
-      <c r="D155" s="6"/>
-      <c r="E155" s="6"/>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
+      <c r="B159" s="7"/>
+      <c r="C159" s="7"/>
+      <c r="D159" s="7"/>
+      <c r="E159" s="7"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B161" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C157" s="2" t="s">
+      <c r="C161" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D157" s="2" t="s">
+      <c r="D161" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="2" t="s">
+      <c r="E161" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C158" s="3">
-        <v>10</v>
-      </c>
-      <c r="D158" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E158" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C159" s="3">
-        <v>20</v>
-      </c>
-      <c r="D159" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E159" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C160" s="3">
-        <v>25</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E160" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C161" s="3">
-        <v>50</v>
-      </c>
-      <c r="D161" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E161" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C162" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="C162" s="3">
+        <v>10</v>
+      </c>
       <c r="D162" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C163" s="3">
+        <v>20</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C164" s="3">
+        <v>25</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" s="3">
+        <v>50</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C166" s="3"/>
+      <c r="D166" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B163" s="3" t="s">
+      <c r="B167" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C163" s="3"/>
-      <c r="D163" s="3" t="s">
+      <c r="C167" s="3"/>
+      <c r="D167" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E163" s="3" t="s">
+      <c r="E167" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="1"/>
-      <c r="B166" s="1"/>
-      <c r="C166" s="1"/>
-      <c r="D166" s="1"/>
-      <c r="E166" s="1"/>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="1"/>
-      <c r="B167" s="1"/>
-      <c r="C167" s="1"/>
-      <c r="D167" s="1"/>
-      <c r="E167" s="1"/>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" s="5"/>
-      <c r="B168" s="5"/>
-      <c r="C168" s="5"/>
-      <c r="D168" s="5"/>
-      <c r="E168" s="5"/>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" s="5"/>
-      <c r="B169" s="5"/>
-      <c r="C169" s="5"/>
-      <c r="D169" s="5"/>
-      <c r="E169" s="5"/>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" s="1"/>
-      <c r="B170" s="1"/>
-      <c r="C170" s="1"/>
-      <c r="D170" s="1"/>
-      <c r="E170" s="1"/>
+    <row r="170" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A170" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B170" s="7"/>
+      <c r="C170" s="7"/>
+      <c r="D170" s="7"/>
+      <c r="E170" s="7"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C173" s="3">
+        <v>10</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C174" s="3">
+        <v>10</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C175" s="3">
+        <v>10</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C176" s="3"/>
+      <c r="D176" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C177" s="3"/>
+      <c r="D177" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A131:E131"/>
-    <mergeCell ref="A144:E144"/>
-    <mergeCell ref="A155:E155"/>
+  <mergeCells count="15">
+    <mergeCell ref="A170:E170"/>
+    <mergeCell ref="A135:E135"/>
+    <mergeCell ref="A148:E148"/>
+    <mergeCell ref="A159:E159"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="A63:E63"/>

</xml_diff>

<commit_message>
add testimonial and slider
</commit_message>
<xml_diff>
--- a/ecommerce.xlsx
+++ b/ecommerce.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31BFF8A-31C4-411C-B0BD-2B7E2C42B952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AE162C-6BAF-4A50-8668-40133B64BFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="2085" windowWidth="7395" windowHeight="7875" xr2:uid="{785BB870-0898-4C38-870A-8BD1466B9A97}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{785BB870-0898-4C38-870A-8BD1466B9A97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -847,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B9B093-5896-4E4E-AD3A-F02ED3F94AD7}">
   <dimension ref="A1:E213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="B214" sqref="B214"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140:E140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3401,6 +3401,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A194:E194"/>
+    <mergeCell ref="A206:E206"/>
+    <mergeCell ref="A184:E184"/>
+    <mergeCell ref="A135:E135"/>
+    <mergeCell ref="A162:E162"/>
+    <mergeCell ref="A173:E173"/>
+    <mergeCell ref="A149:E149"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="A63:E63"/>
@@ -3412,13 +3419,6 @@
     <mergeCell ref="A102:E102"/>
     <mergeCell ref="A111:E111"/>
     <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A194:E194"/>
-    <mergeCell ref="A206:E206"/>
-    <mergeCell ref="A184:E184"/>
-    <mergeCell ref="A135:E135"/>
-    <mergeCell ref="A162:E162"/>
-    <mergeCell ref="A173:E173"/>
-    <mergeCell ref="A149:E149"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add global search bar and product review
</commit_message>
<xml_diff>
--- a/ecommerce.xlsx
+++ b/ecommerce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AE162C-6BAF-4A50-8668-40133B64BFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2579371-2578-474A-826F-4842CA326536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{785BB870-0898-4C38-870A-8BD1466B9A97}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="130">
   <si>
     <t>int</t>
   </si>
@@ -418,6 +418,24 @@
   </si>
   <si>
     <t>Table :-Slider</t>
+  </si>
+  <si>
+    <t>Table :-Product Review</t>
+  </si>
+  <si>
+    <t>Product_Rate</t>
+  </si>
+  <si>
+    <t>Product_Review</t>
+  </si>
+  <si>
+    <t>Table :-All NewsLetter</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Table :- NewsLetter User</t>
   </si>
 </sst>
 </file>
@@ -845,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B9B093-5896-4E4E-AD3A-F02ED3F94AD7}">
-  <dimension ref="A1:E213"/>
+  <dimension ref="A1:E242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140:E140"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="A234" sqref="A234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3399,15 +3417,320 @@
         <v>122</v>
       </c>
     </row>
+    <row r="216" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A216" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B216" s="9"/>
+      <c r="C216" s="9"/>
+      <c r="D216" s="9"/>
+      <c r="E216" s="9"/>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E218" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C219" s="3">
+        <v>10</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B220" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C220" s="5">
+        <v>10</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B221" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C221" s="5">
+        <v>10</v>
+      </c>
+      <c r="D221" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E221" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B222" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C222" s="5">
+        <v>255</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E222" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C223" s="3"/>
+      <c r="D223" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E223" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C224" s="3"/>
+      <c r="D224" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E224" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A227" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B227" s="9"/>
+      <c r="C227" s="9"/>
+      <c r="D227" s="9"/>
+      <c r="E227" s="9"/>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D229" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E229" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C230" s="3">
+        <v>10</v>
+      </c>
+      <c r="D230" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B231" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C231" s="5">
+        <v>50</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E231" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B232" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C232" s="5">
+        <v>255</v>
+      </c>
+      <c r="D232" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E232" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C233" s="3"/>
+      <c r="D233" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C234" s="3"/>
+      <c r="D234" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A237" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B237" s="9"/>
+      <c r="C237" s="9"/>
+      <c r="D237" s="9"/>
+      <c r="E237" s="9"/>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D239" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E239" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C240" s="3">
+        <v>10</v>
+      </c>
+      <c r="D240" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E240" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B241" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C241" s="5">
+        <v>50</v>
+      </c>
+      <c r="D241" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E241" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C242" s="3"/>
+      <c r="D242" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E242" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A194:E194"/>
-    <mergeCell ref="A206:E206"/>
-    <mergeCell ref="A184:E184"/>
-    <mergeCell ref="A135:E135"/>
+  <mergeCells count="21">
     <mergeCell ref="A162:E162"/>
     <mergeCell ref="A173:E173"/>
     <mergeCell ref="A149:E149"/>
+    <mergeCell ref="A227:E227"/>
+    <mergeCell ref="A237:E237"/>
+    <mergeCell ref="A216:E216"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="A63:E63"/>
@@ -3419,6 +3742,10 @@
     <mergeCell ref="A102:E102"/>
     <mergeCell ref="A111:E111"/>
     <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A194:E194"/>
+    <mergeCell ref="A206:E206"/>
+    <mergeCell ref="A184:E184"/>
+    <mergeCell ref="A135:E135"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>